<commit_message>
Add: development file with adjustment solutions
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\ncharnulal-bethaleft-dungeon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{9C808C47-075F-4C29-8C5B-6C76D4C61D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6011AE-75D7-4C29-BB99-D49199FB0EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="8" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -171,12 +171,6 @@
     <t>tlvnbd_gen_l</t>
   </si>
   <si>
-    <t>Small Crystal Extractor</t>
-  </si>
-  <si>
-    <t>Crystal Extractor</t>
-  </si>
-  <si>
     <t>tlvnbd_crystal_deposit</t>
   </si>
   <si>
@@ -199,6 +193,12 @@
   </si>
   <si>
     <t>Kamdida deposit</t>
+  </si>
+  <si>
+    <t>Kamdida Coherer</t>
+  </si>
+  <si>
+    <t>Small Kamdida Coherer</t>
   </si>
 </sst>
 </file>
@@ -2984,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2992,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3016,7 +3016,7 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3358,7 +3358,7 @@
   <dimension ref="A2:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3397,7 +3397,7 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -3411,7 +3411,7 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3422,10 +3422,10 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3433,10 +3433,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update: clean up and placing gen01 pipes
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\ncharnulal-bethaleft-dungeon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B6011AE-75D7-4C29-BB99-D49199FB0EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F409453A-8ADE-43C4-8CF3-C8C8FCFD5CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="8" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -195,10 +195,37 @@
     <t>Kamdida deposit</t>
   </si>
   <si>
-    <t>Kamdida Coherer</t>
-  </si>
-  <si>
-    <t>Small Kamdida Coherer</t>
+    <t>Small Kamdida Dynamo</t>
+  </si>
+  <si>
+    <t>Kamdida Dynamo</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_01</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_01</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_01_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_01_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_Gen_01_State</t>
+  </si>
+  <si>
+    <t>tlvnbd_Gen_02_State</t>
+  </si>
+  <si>
+    <t>tlvnbd_Gen_03_State</t>
+  </si>
+  <si>
+    <t>Handle activation from tlvnbd_Gen_01_State</t>
+  </si>
+  <si>
+    <t>Handle activation &amp; switch tlvnbd_Gen_01_state</t>
   </si>
 </sst>
 </file>
@@ -1303,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:E32"/>
+  <dimension ref="A2:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,9 +1341,10 @@
     <col min="2" max="2" width="35.44140625" customWidth="1"/>
     <col min="4" max="4" width="35.44140625" customWidth="1"/>
     <col min="5" max="5" width="66.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="41.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,31 +1358,58 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
         <v>0</v>
       </c>
@@ -1362,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
         <v>0</v>
       </c>
@@ -1370,7 +1425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
         <v>0</v>
       </c>
@@ -1378,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>0</v>
       </c>
@@ -1386,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>0</v>
       </c>
@@ -1394,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
         <v>0</v>
       </c>
@@ -1402,7 +1457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
         <v>0</v>
       </c>
@@ -1410,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="b">
         <v>0</v>
       </c>
@@ -1418,7 +1473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
         <v>0</v>
       </c>
@@ -1426,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="b">
         <v>0</v>
       </c>
@@ -1434,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
         <v>0</v>
       </c>
@@ -3355,10 +3410,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F94C72C-6EBC-4A19-A0BC-385E0AA67890}">
-  <dimension ref="A2:D32"/>
+  <dimension ref="A2:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3391,13 +3446,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -3405,10 +3457,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
         <v>49</v>
@@ -3422,10 +3474,13 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3433,21 +3488,36 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
@@ -3564,8 +3634,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D32">
+  <conditionalFormatting sqref="B3:D34">
     <cfRule type="expression" dxfId="4" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -3574,7 +3654,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B32" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B34" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3584,7 +3664,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D100</xm:sqref>
+          <xm:sqref>D3:D102</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add: Crystal Processing cell layout & initial piping
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\ncharnulal-bethaleft-dungeon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D1057B-0A42-40B6-BF38-A90F7659F920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CAE601-D368-4D77-A636-3463828547C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="8" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -207,9 +207,6 @@
     <t>tlvnbd_gen_01</t>
   </si>
   <si>
-    <t>tlvnbd_gen_01_sc</t>
-  </si>
-  <si>
     <t>tlvnbd_pipe_gen_01_sc</t>
   </si>
   <si>
@@ -238,6 +235,75 @@
   </si>
   <si>
     <t>tlvnbd_light_kamdida_256</t>
+  </si>
+  <si>
+    <t>tlvnbd_ind_gen_01</t>
+  </si>
+  <si>
+    <t>tlvnbd_ind_gen_01_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_load_gen_01</t>
+  </si>
+  <si>
+    <t>Steel and Iron Dwemer Doors</t>
+  </si>
+  <si>
+    <t>Door</t>
+  </si>
+  <si>
+    <t>tlvnbd_load_gen_0?</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_s_02</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_s_01</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_02</t>
+  </si>
+  <si>
+    <t>tlvnbd_Gen_02a_State</t>
+  </si>
+  <si>
+    <t>tlvnbd_Gen_02b_State</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_02_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_02a_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_02b_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_02a</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_02b</t>
+  </si>
+  <si>
+    <t>tlvnbd_ind_gen_02b</t>
+  </si>
+  <si>
+    <t>tlvnbd_ind_gen_02b_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_s_01_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_s_02_sc</t>
+  </si>
+  <si>
+    <t>ART REQ</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_t_switch_gen_02</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_t_switch_gen_02_sc</t>
   </si>
 </sst>
 </file>
@@ -301,7 +367,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1112,7 +1220,7 @@
   <dimension ref="A2:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1181,7 +1289,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
@@ -1329,10 +1437,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E32">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$A3=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1342,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:F32"/>
+  <dimension ref="A2:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1375,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="4" t="b">
         <v>0</v>
@@ -1384,89 +1492,140 @@
         <v>51</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
       <c r="C4" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="D5" t="s">
+        <v>77</v>
+      </c>
       <c r="F5" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
       <c r="C7" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
       <c r="C8" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
       <c r="C9" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
       <c r="C11" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1637,20 +1796,69 @@
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:E32">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="B12:E37 B10:C11 E10:E11 B3:E9">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$C3=TRUE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B3:B32" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
+  <conditionalFormatting sqref="D10:D11">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$A10=FALSE</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$A10=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B3:B37" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="D10:D11" xr:uid="{A8BEF013-FFC0-481F-88AF-4B9D4D96B775}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1660,7 +1868,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C33:C60</xm:sqref>
+          <xm:sqref>C38:C65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1889,10 +2097,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:C32">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2084,13 +2292,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F32">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$F3="END"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
+    <cfRule type="expression" dxfId="18" priority="2">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2620,10 +2828,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F96">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="16" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2813,10 +3021,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D32">
-    <cfRule type="expression" dxfId="12" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3005,10 +3213,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D32">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3213,10 +3421,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D32">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3406,10 +3614,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D32">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3422,10 +3630,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F94C72C-6EBC-4A19-A0BC-385E0AA67890}">
-  <dimension ref="A2:E34"/>
+  <dimension ref="A2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3472,10 +3680,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
@@ -3483,13 +3688,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -3497,13 +3699,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
@@ -3514,27 +3713,27 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
-        <v>60</v>
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -3542,10 +3741,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>61</v>
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -3553,113 +3755,191 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" t="s">
-        <v>61</v>
+        <v>69</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="b">
         <v>0</v>
       </c>
@@ -3674,17 +3954,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D34">
-    <cfRule type="expression" dxfId="4" priority="1">
+  <conditionalFormatting sqref="B3:D42">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B34" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B42" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3694,7 +4014,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D102</xm:sqref>
+          <xm:sqref>D3:D110</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add: new pipe switch to Gen02 junction
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\ncharnulal-bethaleft-dungeon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CAE601-D368-4D77-A636-3463828547C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39855289-E2F3-4075-9F69-61CA75D8C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="9" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="8" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
   <sheets>
     <sheet name="Cells" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -297,13 +297,19 @@
     <t>tlvnbd_gen_s_02_sc</t>
   </si>
   <si>
-    <t>ART REQ</t>
-  </si>
-  <si>
     <t>tlvnbd_pipe_t_switch_gen_02</t>
   </si>
   <si>
     <t>tlvnbd_pipe_t_switch_gen_02_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_btn_t_switch_gen_02</t>
+  </si>
+  <si>
+    <t>Dwemer Button</t>
+  </si>
+  <si>
+    <t>tlvnbd_btn_t_switch_gen_02_sc</t>
   </si>
 </sst>
 </file>
@@ -1450,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:F37"/>
+  <dimension ref="A2:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1551,16 +1557,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
         <v>56</v>
@@ -1568,19 +1574,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1588,52 +1591,61 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>63</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B12" t="s">
+        <v>80</v>
+      </c>
       <c r="C12" s="4" t="b">
         <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1836,8 +1848,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C38" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B12:E37 B10:C11 E10:E11 B3:E9">
+  <conditionalFormatting sqref="B3:E10 B11:C12 E11:E12 B13:E38">
     <cfRule type="expression" dxfId="4" priority="3">
       <formula>$C3=TRUE</formula>
     </cfRule>
@@ -1848,17 +1868,17 @@
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="D11:D12">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$A10=FALSE</formula>
+      <formula>$A11=FALSE</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$A10=TRUE</formula>
+      <formula>$A11=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B3:B37" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="D10:D11" xr:uid="{A8BEF013-FFC0-481F-88AF-4B9D4D96B775}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B3:B38" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="D11:D12" xr:uid="{A8BEF013-FFC0-481F-88AF-4B9D4D96B775}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1868,7 +1888,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C38:C65</xm:sqref>
+          <xm:sqref>C39:C66</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3630,10 +3650,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F94C72C-6EBC-4A19-A0BC-385E0AA67890}">
-  <dimension ref="A2:E42"/>
+  <dimension ref="A2:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3642,7 +3662,7 @@
     <col min="4" max="4" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3653,7 +3673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
         <v>0</v>
       </c>
@@ -3664,7 +3684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
         <v>1</v>
       </c>
@@ -3675,7 +3695,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
         <v>1</v>
       </c>
@@ -3686,7 +3706,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
         <v>1</v>
       </c>
@@ -3697,7 +3717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
         <v>1</v>
       </c>
@@ -3708,40 +3728,37 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
         <v>49</v>
@@ -3750,12 +3767,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
         <v>49</v>
@@ -3764,26 +3781,26 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -3792,37 +3809,37 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -3830,7 +3847,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>48</v>
@@ -3841,13 +3858,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3855,7 +3875,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>60</v>
@@ -3863,16 +3883,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -3880,7 +3897,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>66</v>
@@ -3893,6 +3910,15 @@
       <c r="A22" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="b">
@@ -3994,8 +4020,13 @@
         <v>0</v>
       </c>
     </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D42">
+  <conditionalFormatting sqref="B3:D43">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4004,7 +4035,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B42" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B43" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4014,7 +4045,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D110</xm:sqref>
+          <xm:sqref>D3:D111</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add: gen s 03 to proc wing
Add: some clutter to proc wing
</commit_message>
<xml_diff>
--- a/Docs/Project Manager.xlsx
+++ b/Docs/Project Manager.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etste\Documents\Projects\Mods\Morrowind\ncharnulal-bethaleft-dungeon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E05A21-73D5-4E15-8C8C-A586AAEC6F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBD18D6-7E0D-4A7D-8F00-B596DE128D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="765" activeTab="8" xr2:uid="{4904B981-F0B7-4F9A-A77B-E04B97902615}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -337,13 +337,34 @@
   </si>
   <si>
     <t>tlvnbd_ind_gen_02a_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_s_03</t>
+  </si>
+  <si>
+    <t>tlvnbd_gen_s_03_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_03</t>
+  </si>
+  <si>
+    <t>tlvnbd_pipe_gen_03_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_light_pipe_gen_02</t>
+  </si>
+  <si>
+    <t>tlvnbd_light_pipe_gen_02_sc</t>
+  </si>
+  <si>
+    <t>tlvnbd_light_pipe_96_falloff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,13 +380,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -380,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -396,6 +435,9 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1525,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC67FCD2-9BDF-478C-9239-4C7EFBA33647}">
-  <dimension ref="A2:F39"/>
+  <dimension ref="A2:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1569,7 +1611,7 @@
       <c r="E3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1586,7 +1628,7 @@
       <c r="D4" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="5" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1603,7 +1645,7 @@
       <c r="D5" t="s">
         <v>74</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1620,7 +1662,7 @@
       <c r="D6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1629,15 +1671,15 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1646,44 +1688,45 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C8" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C9" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1691,16 +1734,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C11" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1708,13 +1748,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C12" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1722,30 +1762,30 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C13" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>61</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C14" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1753,16 +1793,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C15" s="4" t="b">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1770,57 +1807,81 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="b">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="b">
         <v>0</v>
       </c>
@@ -1828,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="b">
         <v>0</v>
       </c>
@@ -1836,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="b">
         <v>0</v>
       </c>
@@ -1844,7 +1905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="b">
         <v>0</v>
       </c>
@@ -1852,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="b">
         <v>0</v>
       </c>
@@ -1860,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="b">
         <v>0</v>
       </c>
@@ -1868,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="b">
         <v>0</v>
       </c>
@@ -1876,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="b">
         <v>0</v>
       </c>
@@ -1884,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="b">
         <v>0</v>
       </c>
@@ -1892,7 +1953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="b">
         <v>0</v>
       </c>
@@ -1900,7 +1961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="b">
         <v>0</v>
       </c>
@@ -1908,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="b">
         <v>0</v>
       </c>
@@ -1972,16 +2033,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B15:B16">
+  <conditionalFormatting sqref="B18:B19">
     <cfRule type="expression" dxfId="6" priority="1">
-      <formula>$A15=FALSE</formula>
+      <formula>$A18=FALSE</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="2">
-      <formula>$A15=TRUE</formula>
+      <formula>$A18=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:E10 E11:E13 B14:E14 C15:E16 B17:E39 B11:C13">
+  <conditionalFormatting sqref="B13:C16 E13:E16 B17:E17 C18:E19 B20:E42 B3:E12">
     <cfRule type="expression" dxfId="4" priority="7">
       <formula>$C3=TRUE</formula>
     </cfRule>
@@ -1992,17 +2077,17 @@
       <formula>$A3=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11:D13">
+  <conditionalFormatting sqref="D13:D16">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$A11=FALSE</formula>
+      <formula>$A13=FALSE</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="6">
-      <formula>$A11=TRUE</formula>
+      <formula>$A13=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B17:B39 B3:B14" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B15:B16 D11:D13" xr:uid="{A8BEF013-FFC0-481F-88AF-4B9D4D96B775}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Character Length Limit" error="Script ID's are limited to 31 characters in the Construction Set." sqref="B20:B42 B3:B17" xr:uid="{8F3E7C0E-9C6D-49C3-A152-B38AC2F64400}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B18:B19 D13:D16" xr:uid="{A8BEF013-FFC0-481F-88AF-4B9D4D96B775}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2012,7 +2097,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C40:C67</xm:sqref>
+          <xm:sqref>C43:C70</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3774,10 +3859,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F94C72C-6EBC-4A19-A0BC-385E0AA67890}">
-  <dimension ref="A2:E42"/>
+  <dimension ref="A2:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3786,7 +3871,7 @@
     <col min="4" max="4" width="9.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3797,7 +3882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="b">
         <v>1</v>
       </c>
@@ -3808,7 +3893,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="b">
         <v>1</v>
       </c>
@@ -3819,7 +3904,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="b">
         <v>1</v>
       </c>
@@ -3830,7 +3915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="b">
         <v>1</v>
       </c>
@@ -3841,51 +3926,48 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -3894,12 +3976,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>47</v>
@@ -3908,115 +3990,118 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>97</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>57</v>
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
-        <v>57</v>
+        <v>76</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -4024,13 +4109,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
-      </c>
-      <c r="C21" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -4038,13 +4120,10 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -4052,30 +4131,63 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
+        <v>101</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="b">
         <v>0</v>
       </c>
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>94</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -4153,8 +4265,28 @@
         <v>0</v>
       </c>
     </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:D42">
+  <conditionalFormatting sqref="B3:D46">
     <cfRule type="expression" dxfId="8" priority="1">
       <formula>$A3=FALSE</formula>
     </cfRule>
@@ -4163,7 +4295,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B42" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Character Length Limit" prompt="Object ID's are limited to 31 characters in the Construction Set." sqref="B3:B46" xr:uid="{8F929C9F-3D1E-43CF-9098-2127BDEB172D}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4173,7 +4305,7 @@
           <x14:formula1>
             <xm:f>Sheet8!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D110</xm:sqref>
+          <xm:sqref>D3:D114</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>